<commit_message>
added language group columns (primary and secondary)
</commit_message>
<xml_diff>
--- a/data/Language sample frequency.xlsx
+++ b/data/Language sample frequency.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\Documents\Utrecht stuff\Pattern Recognition\Accent-Detection\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE67A146-78C6-48FE-BCE9-EE32B4EAA0CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB3F339-1956-473C-8EFF-1CF09768153D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2955ED82-3F38-426B-B955-560BA7C2C229}"/>
   </bookViews>
@@ -19,9 +19,6 @@
     <definedName name="_xlchart.v1.0" hidden="1">Sheet2!$A$2:$A$230</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Sheet2!$B$1</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Sheet2!$B$2:$B$230</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet2!$A$2:$A$230</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet2!$B$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet2!$B$2:$B$230</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="265">
   <si>
     <t>Row Labels</t>
   </si>
@@ -737,6 +734,108 @@
   </si>
   <si>
     <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Primary language group</t>
+  </si>
+  <si>
+    <t>Secondary language group</t>
+  </si>
+  <si>
+    <t>Indo-European</t>
+  </si>
+  <si>
+    <t>Germanic</t>
+  </si>
+  <si>
+    <t>Uralic</t>
+  </si>
+  <si>
+    <t>Finnic</t>
+  </si>
+  <si>
+    <t>Italic</t>
+  </si>
+  <si>
+    <t>Afro-Asiatic</t>
+  </si>
+  <si>
+    <t>Semitic</t>
+  </si>
+  <si>
+    <t>Sino-Tibetan</t>
+  </si>
+  <si>
+    <t>Chinese</t>
+  </si>
+  <si>
+    <t>Koreanic</t>
+  </si>
+  <si>
+    <t>Balto-Slavic</t>
+  </si>
+  <si>
+    <t>Japonic</t>
+  </si>
+  <si>
+    <t>Turkic</t>
+  </si>
+  <si>
+    <t>Southern Turkic</t>
+  </si>
+  <si>
+    <t>Austro-Asiatic</t>
+  </si>
+  <si>
+    <t>Mon-Khmer</t>
+  </si>
+  <si>
+    <t>Indo-Iranian</t>
+  </si>
+  <si>
+    <t>Austronesian</t>
+  </si>
+  <si>
+    <t>Malayo-Polynesian</t>
+  </si>
+  <si>
+    <t>Kra-Dai</t>
+  </si>
+  <si>
+    <t>Kam-Tai</t>
+  </si>
+  <si>
+    <t>Greek</t>
+  </si>
+  <si>
+    <t>Albanian</t>
+  </si>
+  <si>
+    <t>Dravidian</t>
+  </si>
+  <si>
+    <t>South-Central Dravidian</t>
+  </si>
+  <si>
+    <t>Southern Dravidian</t>
+  </si>
+  <si>
+    <t>Misumalpan</t>
+  </si>
+  <si>
+    <t>Niger-Congo</t>
+  </si>
+  <si>
+    <t>Atlantic-Congo</t>
+  </si>
+  <si>
+    <t>Mongolic</t>
+  </si>
+  <si>
+    <t>Eastern Mongolic</t>
+  </si>
+  <si>
+    <t>Chadic</t>
   </si>
 </sst>
 </file>
@@ -797,10 +896,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -844,7 +943,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{27AA23D7-51B4-4235-98AC-DF70C628331E}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:f>_xlchart.v1.1</cx:f>
               <cx:v>Count of file_name</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1790,7 +1889,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1798,450 +1897,777 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B5C57D-7945-439C-A89A-E2AD558BC2F7}">
-  <dimension ref="A1:B230"/>
+  <dimension ref="A1:D230"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>651</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <v>235</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
         <v>200</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
         <v>156</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>240</v>
+      </c>
+      <c r="D5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
         <v>97</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>242</v>
+      </c>
+      <c r="D6" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7">
         <v>85</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>233</v>
+      </c>
+      <c r="D7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8">
         <v>81</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>233</v>
+      </c>
+      <c r="D8" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
         <v>69</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10">
         <v>54</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>233</v>
+      </c>
+      <c r="D10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11">
         <v>45</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>233</v>
+      </c>
+      <c r="D11" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>244</v>
+      </c>
+      <c r="D12" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13">
         <v>42</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>245</v>
+      </c>
+      <c r="D13" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14">
         <v>40</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>247</v>
+      </c>
+      <c r="D14" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15">
         <v>39</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>233</v>
+      </c>
+      <c r="D15" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16">
         <v>39</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>233</v>
+      </c>
+      <c r="D16" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>233</v>
+      </c>
+      <c r="D17" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>240</v>
+      </c>
+      <c r="D18" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19">
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>233</v>
+      </c>
+      <c r="D19" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>233</v>
+      </c>
+      <c r="D20" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21">
         <v>27</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>250</v>
+      </c>
+      <c r="D21" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22">
         <v>27</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>238</v>
+      </c>
+      <c r="D22" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23">
         <v>27</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>233</v>
+      </c>
+      <c r="D23" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>233</v>
+      </c>
+      <c r="D24" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>252</v>
+      </c>
+      <c r="D25" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>233</v>
+      </c>
+      <c r="D26" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27">
         <v>22</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>233</v>
+      </c>
+      <c r="D27" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
       <c r="B28">
         <v>20</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>233</v>
+      </c>
+      <c r="D28" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
       <c r="B29">
         <v>19</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>233</v>
+      </c>
+      <c r="D29" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30">
         <v>18</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>233</v>
+      </c>
+      <c r="D30" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31">
         <v>17</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>233</v>
+      </c>
+      <c r="D31" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="B32">
         <v>17</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>233</v>
+      </c>
+      <c r="D32" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
       <c r="B33">
         <v>17</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>235</v>
+      </c>
+      <c r="D33" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
       <c r="B34">
         <v>15</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>256</v>
+      </c>
+      <c r="D34" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35">
         <v>15</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>235</v>
+      </c>
+      <c r="D35" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
       <c r="B36">
         <v>14</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>233</v>
+      </c>
+      <c r="D36" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
       <c r="B37">
         <v>14</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>233</v>
+      </c>
+      <c r="D37" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
       <c r="B38">
         <v>14</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>250</v>
+      </c>
+      <c r="D38" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
       <c r="B39">
         <v>13</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>256</v>
+      </c>
+      <c r="D39" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
       <c r="B40">
         <v>13</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>235</v>
+      </c>
+      <c r="D40" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
       <c r="B41">
         <v>13</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>233</v>
+      </c>
+      <c r="D41" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
       <c r="B42">
         <v>12</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>233</v>
+      </c>
+      <c r="D42" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
       <c r="B43">
         <v>12</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>233</v>
+      </c>
+      <c r="D43" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
       <c r="B44">
         <v>11</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>240</v>
+      </c>
+      <c r="D44" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
       <c r="B45">
         <v>11</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>238</v>
+      </c>
+      <c r="D45" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
       <c r="B46">
         <v>11</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>259</v>
+      </c>
+      <c r="D46" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
       <c r="B47">
         <v>11</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>260</v>
+      </c>
+      <c r="D47" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
       <c r="B48">
         <v>11</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>233</v>
+      </c>
+      <c r="D48" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
       <c r="B49">
         <v>10</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>262</v>
+      </c>
+      <c r="D49" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
       <c r="B50">
         <v>10</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>233</v>
+      </c>
+      <c r="D50" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
       <c r="B51">
         <v>10</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>233</v>
+      </c>
+      <c r="D51" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
       <c r="B52">
         <v>10</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>233</v>
+      </c>
+      <c r="D52" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
       <c r="B53">
         <v>10</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>233</v>
+      </c>
+      <c r="D53" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
       <c r="B54">
         <v>10</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>238</v>
+      </c>
+      <c r="D54" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -2249,7 +2675,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -2257,7 +2683,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -2265,7 +2691,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -2273,23 +2699,35 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>59</v>
       </c>
       <c r="B59">
         <v>9</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>233</v>
+      </c>
+      <c r="D59" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>60</v>
       </c>
       <c r="B60">
         <v>9</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>233</v>
+      </c>
+      <c r="D60" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>61</v>
       </c>
@@ -2297,7 +2735,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -2305,7 +2743,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -2313,7 +2751,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -2321,15 +2759,21 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>65</v>
       </c>
       <c r="B65">
         <v>8</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>233</v>
+      </c>
+      <c r="D65" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -2337,15 +2781,21 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>67</v>
       </c>
       <c r="B67">
         <v>8</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>233</v>
+      </c>
+      <c r="D67" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -2353,7 +2803,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>69</v>
       </c>
@@ -2361,7 +2811,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -2369,7 +2819,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -2377,7 +2827,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -2385,23 +2835,35 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>73</v>
       </c>
       <c r="B73">
         <v>6</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>233</v>
+      </c>
+      <c r="D73" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>74</v>
       </c>
       <c r="B74">
         <v>6</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>233</v>
+      </c>
+      <c r="D74" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>75</v>
       </c>
@@ -2409,7 +2871,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>76</v>
       </c>
@@ -2417,23 +2879,35 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>77</v>
       </c>
       <c r="B77">
         <v>6</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>233</v>
+      </c>
+      <c r="D77" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>78</v>
       </c>
       <c r="B78">
         <v>6</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>245</v>
+      </c>
+      <c r="D78" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>79</v>
       </c>
@@ -2441,7 +2915,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>80</v>
       </c>
@@ -2449,7 +2923,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>81</v>
       </c>
@@ -2457,7 +2931,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -2465,7 +2939,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>83</v>
       </c>
@@ -2473,7 +2947,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>84</v>
       </c>
@@ -2481,7 +2955,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>85</v>
       </c>
@@ -2489,7 +2963,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>86</v>
       </c>
@@ -2497,7 +2971,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>87</v>
       </c>
@@ -2505,7 +2979,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>88</v>
       </c>
@@ -2513,7 +2987,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>89</v>
       </c>
@@ -2521,7 +2995,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>90</v>
       </c>
@@ -2529,7 +3003,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>91</v>
       </c>
@@ -2537,7 +3011,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>92</v>
       </c>
@@ -2545,7 +3019,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>93</v>
       </c>
@@ -2553,15 +3027,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>94</v>
       </c>
       <c r="B94">
         <v>3</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C94" t="s">
+        <v>233</v>
+      </c>
+      <c r="D94" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>95</v>
       </c>
@@ -2569,7 +3049,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>96</v>
       </c>
@@ -2577,7 +3057,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>97</v>
       </c>
@@ -2585,7 +3065,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>98</v>
       </c>
@@ -2593,7 +3073,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>99</v>
       </c>
@@ -2601,7 +3081,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>100</v>
       </c>
@@ -2609,7 +3089,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>101</v>
       </c>
@@ -2617,7 +3097,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>102</v>
       </c>
@@ -2625,7 +3105,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>103</v>
       </c>
@@ -2633,7 +3113,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>104</v>
       </c>
@@ -2641,15 +3121,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>105</v>
       </c>
       <c r="B105">
         <v>3</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C105" t="s">
+        <v>233</v>
+      </c>
+      <c r="D105" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>106</v>
       </c>
@@ -2657,7 +3143,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>107</v>
       </c>
@@ -2665,7 +3151,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>108</v>
       </c>
@@ -2673,7 +3159,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>109</v>
       </c>
@@ -2681,7 +3167,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>110</v>
       </c>
@@ -2689,7 +3175,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>111</v>
       </c>
@@ -2697,7 +3183,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>112</v>
       </c>
@@ -2705,7 +3191,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>113</v>
       </c>
@@ -2713,7 +3199,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>114</v>
       </c>
@@ -2721,7 +3207,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>115</v>
       </c>
@@ -2729,7 +3215,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>116</v>
       </c>
@@ -2737,7 +3223,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>117</v>
       </c>
@@ -2745,15 +3231,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>118</v>
       </c>
       <c r="B118">
         <v>2</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C118" t="s">
+        <v>233</v>
+      </c>
+      <c r="D118" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>119</v>
       </c>
@@ -2761,7 +3253,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>120</v>
       </c>
@@ -2769,7 +3261,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>121</v>
       </c>
@@ -2777,7 +3269,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>122</v>
       </c>
@@ -2785,7 +3277,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>123</v>
       </c>
@@ -2793,7 +3285,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>124</v>
       </c>
@@ -2801,7 +3293,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>125</v>
       </c>
@@ -2809,7 +3301,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>126</v>
       </c>
@@ -2817,7 +3309,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>127</v>
       </c>
@@ -2825,12 +3317,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>128</v>
       </c>
       <c r="B128">
         <v>2</v>
+      </c>
+      <c r="C128" t="s">
+        <v>245</v>
+      </c>
+      <c r="D128" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added language group class labels
</commit_message>
<xml_diff>
--- a/data/Language sample frequency.xlsx
+++ b/data/Language sample frequency.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\Documents\Utrecht stuff\Pattern Recognition\Accent-Detection\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB3F339-1956-473C-8EFF-1CF09768153D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D632AC-04F4-46D2-9EA6-F44DBD4BCEF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2955ED82-3F38-426B-B955-560BA7C2C229}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$B$1:$B$231</definedName>
     <definedName name="_xlchart.v1.0" hidden="1">Sheet2!$A$2:$A$230</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Sheet2!$B$1</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Sheet2!$B$2:$B$230</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="267">
   <si>
     <t>Row Labels</t>
   </si>
@@ -836,6 +837,12 @@
   </si>
   <si>
     <t>Chadic</t>
+  </si>
+  <si>
+    <t>primary id</t>
+  </si>
+  <si>
+    <t>secondary id</t>
   </si>
 </sst>
 </file>
@@ -1521,16 +1528,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>390524</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>304799</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>523874</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -1566,7 +1573,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5591174" y="571500"/>
+              <a:off x="12353924" y="1133475"/>
               <a:ext cx="4791075" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1897,10 +1904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B5C57D-7945-439C-A89A-E2AD558BC2F7}">
-  <dimension ref="A1:D230"/>
+  <dimension ref="A1:F230"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1909,9 +1916,10 @@
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="3" width="24.5703125" customWidth="1"/>
     <col min="4" max="4" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1924,139 +1932,187 @@
       <c r="D1" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B2">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>651</v>
-      </c>
-      <c r="C2" t="s">
-        <v>233</v>
-      </c>
-      <c r="D2" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>235</v>
       </c>
       <c r="C3" t="s">
         <v>233</v>
       </c>
       <c r="D3" t="s">
+        <v>234</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>235</v>
+      </c>
+      <c r="C4" t="s">
+        <v>233</v>
+      </c>
+      <c r="D4" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>200</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>238</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>156</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>240</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="E6">
+        <v>12</v>
+      </c>
+      <c r="F6">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>97</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>242</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="E7">
         <v>7</v>
       </c>
-      <c r="B7">
+      <c r="F7">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
         <v>85</v>
-      </c>
-      <c r="C7" t="s">
-        <v>233</v>
-      </c>
-      <c r="D7" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>81</v>
       </c>
       <c r="C8" t="s">
         <v>233</v>
       </c>
       <c r="D8" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="C9" t="s">
         <v>233</v>
       </c>
       <c r="D9" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
         <v>233</v>
       </c>
       <c r="D10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C11" t="s">
         <v>233</v>
@@ -2064,66 +2120,96 @@
       <c r="D11" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>45</v>
       </c>
       <c r="C12" t="s">
+        <v>233</v>
+      </c>
+      <c r="D12" t="s">
+        <v>234</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
         <v>244</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="E13">
+        <v>6</v>
+      </c>
+      <c r="F13">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>42</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>245</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="E14">
+        <v>13</v>
+      </c>
+      <c r="F14">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>40</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>247</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>15</v>
-      </c>
-      <c r="B15">
-        <v>39</v>
-      </c>
-      <c r="C15" t="s">
-        <v>233</v>
-      </c>
-      <c r="D15" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>16</v>
       </c>
       <c r="B16">
         <v>39</v>
@@ -2132,12 +2218,18 @@
         <v>233</v>
       </c>
       <c r="D16" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
+      </c>
+      <c r="F16">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>39</v>
@@ -2146,43 +2238,61 @@
         <v>233</v>
       </c>
       <c r="D17" t="s">
+        <v>249</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>233</v>
+      </c>
+      <c r="D18" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B18">
+      <c r="B19">
         <v>35</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>240</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="E19">
+        <v>12</v>
+      </c>
+      <c r="F19">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B19">
+      <c r="B20">
         <v>34</v>
-      </c>
-      <c r="C19" t="s">
-        <v>233</v>
-      </c>
-      <c r="D19" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20">
-        <v>29</v>
       </c>
       <c r="C20" t="s">
         <v>233</v>
@@ -2190,22 +2300,34 @@
       <c r="D20" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="D21" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="F21">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -2218,50 +2340,74 @@
       <c r="D22" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>27</v>
       </c>
       <c r="C23" t="s">
-        <v>233</v>
+        <v>250</v>
       </c>
       <c r="D23" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
         <v>233</v>
       </c>
       <c r="D24" t="s">
+        <v>243</v>
+      </c>
+      <c r="E24">
+        <v>5</v>
+      </c>
+      <c r="F24">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>233</v>
+      </c>
+      <c r="D25" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25">
-        <v>23</v>
-      </c>
-      <c r="C25" t="s">
-        <v>252</v>
-      </c>
-      <c r="D25" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="F25">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2274,41 +2420,59 @@
       <c r="D26" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="F26">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>23</v>
+      </c>
+      <c r="C27" t="s">
+        <v>252</v>
+      </c>
+      <c r="D27" t="s">
+        <v>253</v>
+      </c>
+      <c r="E27">
+        <v>8</v>
+      </c>
+      <c r="F27">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>27</v>
       </c>
-      <c r="B27">
+      <c r="B28">
         <v>22</v>
-      </c>
-      <c r="C27" t="s">
-        <v>233</v>
-      </c>
-      <c r="D27" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28">
-        <v>20</v>
       </c>
       <c r="C28" t="s">
         <v>233</v>
       </c>
       <c r="D28" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+      <c r="E28">
+        <v>5</v>
+      </c>
+      <c r="F28">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C29" t="s">
         <v>233</v>
@@ -2316,27 +2480,39 @@
       <c r="D29" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>5</v>
+      </c>
+      <c r="F29">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C30" t="s">
         <v>233</v>
       </c>
       <c r="D30" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+      <c r="E30">
+        <v>5</v>
+      </c>
+      <c r="F30">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C31" t="s">
         <v>233</v>
@@ -2344,8 +2520,14 @@
       <c r="D31" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>5</v>
+      </c>
+      <c r="F31">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -2358,120 +2540,174 @@
       <c r="D32" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>5</v>
+      </c>
+      <c r="F32">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B33">
         <v>17</v>
       </c>
       <c r="C33" t="s">
+        <v>233</v>
+      </c>
+      <c r="D33" t="s">
+        <v>249</v>
+      </c>
+      <c r="E33">
+        <v>5</v>
+      </c>
+      <c r="F33">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>17</v>
+      </c>
+      <c r="C34" t="s">
         <v>235</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D34" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="E34">
+        <v>14</v>
+      </c>
+      <c r="F34">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>34</v>
-      </c>
-      <c r="B34">
-        <v>15</v>
-      </c>
-      <c r="C34" t="s">
-        <v>256</v>
-      </c>
-      <c r="D34" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>35</v>
       </c>
       <c r="B35">
         <v>15</v>
       </c>
       <c r="C35" t="s">
+        <v>256</v>
+      </c>
+      <c r="D35" t="s">
+        <v>257</v>
+      </c>
+      <c r="E35">
+        <v>4</v>
+      </c>
+      <c r="F35">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>15</v>
+      </c>
+      <c r="C36" t="s">
         <v>235</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36">
+      <c r="E36">
         <v>14</v>
       </c>
-      <c r="C36" t="s">
-        <v>233</v>
-      </c>
-      <c r="D36" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B37">
         <v>14</v>
       </c>
       <c r="C37" t="s">
-        <v>233</v>
+        <v>250</v>
       </c>
       <c r="D37" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+      <c r="E37">
+        <v>3</v>
+      </c>
+      <c r="F37">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B38">
         <v>14</v>
       </c>
       <c r="C38" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="D38" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+      <c r="E38">
+        <v>5</v>
+      </c>
+      <c r="F38">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>14</v>
+      </c>
+      <c r="C39" t="s">
+        <v>233</v>
+      </c>
+      <c r="D39" t="s">
+        <v>249</v>
+      </c>
+      <c r="E39">
+        <v>5</v>
+      </c>
+      <c r="F39">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>39</v>
-      </c>
-      <c r="B39">
-        <v>13</v>
-      </c>
-      <c r="C39" t="s">
-        <v>256</v>
-      </c>
-      <c r="D39" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>40</v>
       </c>
       <c r="B40">
         <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>235</v>
+        <v>256</v>
       </c>
       <c r="D40" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="E40">
+        <v>4</v>
+      </c>
+      <c r="F40">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -2484,24 +2720,36 @@
       <c r="D41" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>5</v>
+      </c>
+      <c r="F41">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>13</v>
+      </c>
+      <c r="C42" t="s">
+        <v>235</v>
+      </c>
+      <c r="D42" t="s">
+        <v>235</v>
+      </c>
+      <c r="E42">
+        <v>14</v>
+      </c>
+      <c r="F42">
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>42</v>
-      </c>
-      <c r="B42">
-        <v>12</v>
-      </c>
-      <c r="C42" t="s">
-        <v>233</v>
-      </c>
-      <c r="D42" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>43</v>
       </c>
       <c r="B43">
         <v>12</v>
@@ -2510,24 +2758,36 @@
         <v>233</v>
       </c>
       <c r="D43" t="s">
+        <v>243</v>
+      </c>
+      <c r="E43">
+        <v>5</v>
+      </c>
+      <c r="F43">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>12</v>
+      </c>
+      <c r="C44" t="s">
+        <v>233</v>
+      </c>
+      <c r="D44" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44">
-        <v>11</v>
-      </c>
-      <c r="C44" t="s">
-        <v>240</v>
-      </c>
-      <c r="D44" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <v>5</v>
+      </c>
+      <c r="F44">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -2540,80 +2800,116 @@
       <c r="D45" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B46">
         <v>11</v>
       </c>
       <c r="C46" t="s">
-        <v>259</v>
+        <v>233</v>
       </c>
       <c r="D46" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+      <c r="E46">
+        <v>5</v>
+      </c>
+      <c r="F46">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B47">
         <v>11</v>
       </c>
       <c r="C47" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D47" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+      <c r="E47">
+        <v>9</v>
+      </c>
+      <c r="F47">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48">
         <v>11</v>
       </c>
       <c r="C48" t="s">
-        <v>233</v>
+        <v>260</v>
       </c>
       <c r="D48" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+      <c r="E48">
+        <v>11</v>
+      </c>
+      <c r="F48">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B49">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C49" t="s">
-        <v>262</v>
+        <v>240</v>
       </c>
       <c r="D49" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+      <c r="E49">
+        <v>12</v>
+      </c>
+      <c r="F49">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B50">
         <v>10</v>
       </c>
       <c r="C50" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="D50" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B51">
         <v>10</v>
@@ -2624,10 +2920,16 @@
       <c r="D51" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <v>5</v>
+      </c>
+      <c r="F51">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B52">
         <v>10</v>
@@ -2638,10 +2940,16 @@
       <c r="D52" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <v>5</v>
+      </c>
+      <c r="F52">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53">
         <v>10</v>
@@ -2652,190 +2960,328 @@
       <c r="D53" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53">
+        <v>5</v>
+      </c>
+      <c r="F53">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B54">
         <v>10</v>
       </c>
       <c r="C54" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D54" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+      <c r="E54">
+        <v>5</v>
+      </c>
+      <c r="F54">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B55">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="C55" t="s">
+        <v>262</v>
+      </c>
+      <c r="D55" t="s">
+        <v>263</v>
+      </c>
+      <c r="E55">
+        <v>10</v>
+      </c>
+      <c r="F55">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B56">
         <v>9</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>233</v>
+      </c>
+      <c r="D56" t="s">
+        <v>243</v>
+      </c>
+      <c r="E56">
+        <v>5</v>
+      </c>
+      <c r="F56">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B57">
         <v>9</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>233</v>
+      </c>
+      <c r="D57" t="s">
+        <v>234</v>
+      </c>
+      <c r="E57">
+        <v>5</v>
+      </c>
+      <c r="F57">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B58">
         <v>9</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B59">
         <v>9</v>
       </c>
-      <c r="C59" t="s">
-        <v>233</v>
-      </c>
-      <c r="D59" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B60">
         <v>9</v>
       </c>
-      <c r="C60" t="s">
-        <v>233</v>
-      </c>
-      <c r="D60" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B61">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B62">
         <v>8</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>233</v>
+      </c>
+      <c r="D62" t="s">
+        <v>243</v>
+      </c>
+      <c r="E62">
+        <v>5</v>
+      </c>
+      <c r="F62">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B63">
         <v>8</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>233</v>
+      </c>
+      <c r="D63" t="s">
+        <v>243</v>
+      </c>
+      <c r="E63">
+        <v>5</v>
+      </c>
+      <c r="F63">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B64">
         <v>8</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B65">
         <v>8</v>
       </c>
-      <c r="C65" t="s">
-        <v>233</v>
-      </c>
-      <c r="D65" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B66">
         <v>8</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B67">
         <v>8</v>
       </c>
-      <c r="C67" t="s">
-        <v>233</v>
-      </c>
-      <c r="D67" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <v>8</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>68</v>
-      </c>
-      <c r="B68">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>69</v>
       </c>
       <c r="B69">
         <v>7</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B70">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B71">
         <v>6</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>233</v>
+      </c>
+      <c r="D71" t="s">
+        <v>243</v>
+      </c>
+      <c r="E71">
+        <v>5</v>
+      </c>
+      <c r="F71">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B72">
         <v>6</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>233</v>
+      </c>
+      <c r="D72" t="s">
+        <v>234</v>
+      </c>
+      <c r="E72">
+        <v>5</v>
+      </c>
+      <c r="F72">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -2848,1306 +3294,2247 @@
       <c r="D73" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73">
+        <v>5</v>
+      </c>
+      <c r="F73">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B74">
         <v>6</v>
       </c>
       <c r="C74" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="D74" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+      <c r="E74">
+        <v>13</v>
+      </c>
+      <c r="F74">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B75">
         <v>6</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B76">
         <v>6</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B77">
         <v>6</v>
       </c>
-      <c r="C77" t="s">
-        <v>233</v>
-      </c>
-      <c r="D77" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B78">
         <v>6</v>
       </c>
-      <c r="C78" t="s">
-        <v>245</v>
-      </c>
-      <c r="D78" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B79">
         <v>6</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B80">
         <v>6</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B81">
         <v>6</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <v>6</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>82</v>
-      </c>
-      <c r="B82">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>83</v>
       </c>
       <c r="B83">
         <v>5</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B84">
         <v>5</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B85">
         <v>5</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B86">
         <v>5</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="F86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>86</v>
+      </c>
+      <c r="B87">
+        <v>5</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>87</v>
-      </c>
-      <c r="B87">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>88</v>
       </c>
       <c r="B88">
         <v>4</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B89">
         <v>4</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89">
+        <v>0</v>
+      </c>
+      <c r="F89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B90">
         <v>4</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="F90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B91">
         <v>4</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E91">
+        <v>0</v>
+      </c>
+      <c r="F91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B92">
         <v>4</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92">
+        <v>0</v>
+      </c>
+      <c r="F92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B93">
         <v>4</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93">
+        <v>0</v>
+      </c>
+      <c r="F93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>93</v>
+      </c>
+      <c r="B94">
+        <v>4</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="F94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>94</v>
-      </c>
-      <c r="B94">
-        <v>3</v>
-      </c>
-      <c r="C94" t="s">
-        <v>233</v>
-      </c>
-      <c r="D94" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>95</v>
       </c>
       <c r="B95">
         <v>3</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C95" t="s">
+        <v>233</v>
+      </c>
+      <c r="D95" t="s">
+        <v>243</v>
+      </c>
+      <c r="E95">
+        <v>5</v>
+      </c>
+      <c r="F95">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="B96">
         <v>3</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C96" t="s">
+        <v>233</v>
+      </c>
+      <c r="D96" t="s">
+        <v>243</v>
+      </c>
+      <c r="E96">
+        <v>5</v>
+      </c>
+      <c r="F96">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B97">
         <v>3</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B98">
         <v>3</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E98">
+        <v>0</v>
+      </c>
+      <c r="F98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B99">
         <v>3</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99">
+        <v>0</v>
+      </c>
+      <c r="F99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B100">
         <v>3</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100">
+        <v>0</v>
+      </c>
+      <c r="F100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B101">
         <v>3</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E101">
+        <v>0</v>
+      </c>
+      <c r="F101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B102">
         <v>3</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E102">
+        <v>0</v>
+      </c>
+      <c r="F102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B103">
         <v>3</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E103">
+        <v>0</v>
+      </c>
+      <c r="F103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B104">
         <v>3</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E104">
+        <v>0</v>
+      </c>
+      <c r="F104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B105">
         <v>3</v>
       </c>
-      <c r="C105" t="s">
-        <v>233</v>
-      </c>
-      <c r="D105" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E105">
+        <v>0</v>
+      </c>
+      <c r="F105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B106">
         <v>3</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E106">
+        <v>0</v>
+      </c>
+      <c r="F106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B107">
         <v>3</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E107">
+        <v>0</v>
+      </c>
+      <c r="F107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B108">
         <v>3</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E108">
+        <v>0</v>
+      </c>
+      <c r="F108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B109">
         <v>3</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E109">
+        <v>0</v>
+      </c>
+      <c r="F109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B110">
         <v>3</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E110">
+        <v>0</v>
+      </c>
+      <c r="F110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B111">
         <v>3</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E111">
+        <v>0</v>
+      </c>
+      <c r="F111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B112">
         <v>3</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E112">
+        <v>0</v>
+      </c>
+      <c r="F112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B113">
         <v>3</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E113">
+        <v>0</v>
+      </c>
+      <c r="F113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B114">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="E114">
+        <v>0</v>
+      </c>
+      <c r="F114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B115">
         <v>2</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C115" t="s">
+        <v>233</v>
+      </c>
+      <c r="D115" t="s">
+        <v>243</v>
+      </c>
+      <c r="E115">
+        <v>5</v>
+      </c>
+      <c r="F115">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="B116">
         <v>2</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C116" t="s">
+        <v>245</v>
+      </c>
+      <c r="D116" t="s">
+        <v>246</v>
+      </c>
+      <c r="E116">
+        <v>13</v>
+      </c>
+      <c r="F116">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B117">
         <v>2</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E117">
+        <v>0</v>
+      </c>
+      <c r="F117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B118">
         <v>2</v>
       </c>
-      <c r="C118" t="s">
-        <v>233</v>
-      </c>
-      <c r="D118" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E118">
+        <v>0</v>
+      </c>
+      <c r="F118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B119">
         <v>2</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E119">
+        <v>0</v>
+      </c>
+      <c r="F119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B120">
         <v>2</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E120">
+        <v>0</v>
+      </c>
+      <c r="F120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B121">
         <v>2</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E121">
+        <v>0</v>
+      </c>
+      <c r="F121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B122">
         <v>2</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E122">
+        <v>0</v>
+      </c>
+      <c r="F122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B123">
         <v>2</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E123">
+        <v>0</v>
+      </c>
+      <c r="F123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B124">
         <v>2</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E124">
+        <v>0</v>
+      </c>
+      <c r="F124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B125">
         <v>2</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E125">
+        <v>0</v>
+      </c>
+      <c r="F125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B126">
         <v>2</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E126">
+        <v>0</v>
+      </c>
+      <c r="F126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B127">
         <v>2</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E127">
+        <v>0</v>
+      </c>
+      <c r="F127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B128">
         <v>2</v>
       </c>
-      <c r="C128" t="s">
-        <v>245</v>
-      </c>
-      <c r="D128" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E128">
+        <v>0</v>
+      </c>
+      <c r="F128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B129">
         <v>2</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E129">
+        <v>0</v>
+      </c>
+      <c r="F129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B130">
         <v>2</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E130">
+        <v>0</v>
+      </c>
+      <c r="F130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B131">
         <v>2</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E131">
+        <v>0</v>
+      </c>
+      <c r="F131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B132">
         <v>2</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E132">
+        <v>0</v>
+      </c>
+      <c r="F132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B133">
         <v>2</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E133">
+        <v>0</v>
+      </c>
+      <c r="F133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B134">
         <v>2</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E134">
+        <v>0</v>
+      </c>
+      <c r="F134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B135">
         <v>2</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E135">
+        <v>0</v>
+      </c>
+      <c r="F135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B136">
         <v>2</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E136">
+        <v>0</v>
+      </c>
+      <c r="F136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B137">
         <v>2</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E137">
+        <v>0</v>
+      </c>
+      <c r="F137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B138">
         <v>2</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E138">
+        <v>0</v>
+      </c>
+      <c r="F138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B139">
         <v>2</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E139">
+        <v>0</v>
+      </c>
+      <c r="F139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B140">
         <v>2</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E140">
+        <v>0</v>
+      </c>
+      <c r="F140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B141">
         <v>2</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E141">
+        <v>0</v>
+      </c>
+      <c r="F141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B142">
         <v>2</v>
       </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E142">
+        <v>0</v>
+      </c>
+      <c r="F142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B143">
         <v>2</v>
       </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E143">
+        <v>0</v>
+      </c>
+      <c r="F143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B144">
         <v>2</v>
       </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E144">
+        <v>0</v>
+      </c>
+      <c r="F144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
+        <v>144</v>
+      </c>
+      <c r="B145">
+        <v>2</v>
+      </c>
+      <c r="E145">
+        <v>0</v>
+      </c>
+      <c r="F145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>145</v>
       </c>
-      <c r="B145">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
+      <c r="B146">
+        <v>1</v>
+      </c>
+      <c r="E146">
+        <v>0</v>
+      </c>
+      <c r="F146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
         <v>146</v>
       </c>
-      <c r="B146">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+      <c r="B147">
+        <v>1</v>
+      </c>
+      <c r="E147">
+        <v>0</v>
+      </c>
+      <c r="F147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>147</v>
       </c>
-      <c r="B147">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+      <c r="B148">
+        <v>1</v>
+      </c>
+      <c r="E148">
+        <v>0</v>
+      </c>
+      <c r="F148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>148</v>
       </c>
-      <c r="B148">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+      <c r="B149">
+        <v>1</v>
+      </c>
+      <c r="E149">
+        <v>0</v>
+      </c>
+      <c r="F149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>149</v>
       </c>
-      <c r="B149">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
+      <c r="B150">
+        <v>1</v>
+      </c>
+      <c r="E150">
+        <v>0</v>
+      </c>
+      <c r="F150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>150</v>
       </c>
-      <c r="B150">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+      <c r="B151">
+        <v>1</v>
+      </c>
+      <c r="E151">
+        <v>0</v>
+      </c>
+      <c r="F151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
         <v>151</v>
       </c>
-      <c r="B151">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
+      <c r="B152">
+        <v>1</v>
+      </c>
+      <c r="E152">
+        <v>0</v>
+      </c>
+      <c r="F152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
         <v>152</v>
       </c>
-      <c r="B152">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
+      <c r="B153">
+        <v>1</v>
+      </c>
+      <c r="E153">
+        <v>0</v>
+      </c>
+      <c r="F153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
         <v>153</v>
       </c>
-      <c r="B153">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
+      <c r="B154">
+        <v>1</v>
+      </c>
+      <c r="E154">
+        <v>0</v>
+      </c>
+      <c r="F154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
         <v>154</v>
       </c>
-      <c r="B154">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+      <c r="B155">
+        <v>1</v>
+      </c>
+      <c r="E155">
+        <v>0</v>
+      </c>
+      <c r="F155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
         <v>155</v>
       </c>
-      <c r="B155">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
+      <c r="B156">
+        <v>1</v>
+      </c>
+      <c r="E156">
+        <v>0</v>
+      </c>
+      <c r="F156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
         <v>156</v>
       </c>
-      <c r="B156">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
+      <c r="B157">
+        <v>1</v>
+      </c>
+      <c r="E157">
+        <v>0</v>
+      </c>
+      <c r="F157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
         <v>157</v>
       </c>
-      <c r="B157">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
+      <c r="B158">
+        <v>1</v>
+      </c>
+      <c r="E158">
+        <v>0</v>
+      </c>
+      <c r="F158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
         <v>158</v>
       </c>
-      <c r="B158">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
+      <c r="B159">
+        <v>1</v>
+      </c>
+      <c r="E159">
+        <v>0</v>
+      </c>
+      <c r="F159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
         <v>159</v>
       </c>
-      <c r="B159">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
+      <c r="B160">
+        <v>1</v>
+      </c>
+      <c r="E160">
+        <v>0</v>
+      </c>
+      <c r="F160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
         <v>160</v>
       </c>
-      <c r="B160">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
+      <c r="B161">
+        <v>1</v>
+      </c>
+      <c r="E161">
+        <v>0</v>
+      </c>
+      <c r="F161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
         <v>161</v>
       </c>
-      <c r="B161">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
+      <c r="B162">
+        <v>1</v>
+      </c>
+      <c r="E162">
+        <v>0</v>
+      </c>
+      <c r="F162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
         <v>162</v>
       </c>
-      <c r="B162">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
+      <c r="B163">
+        <v>1</v>
+      </c>
+      <c r="E163">
+        <v>0</v>
+      </c>
+      <c r="F163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
         <v>163</v>
       </c>
-      <c r="B163">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
+      <c r="B164">
+        <v>1</v>
+      </c>
+      <c r="E164">
+        <v>0</v>
+      </c>
+      <c r="F164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
         <v>164</v>
       </c>
-      <c r="B164">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
+      <c r="B165">
+        <v>1</v>
+      </c>
+      <c r="E165">
+        <v>0</v>
+      </c>
+      <c r="F165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
         <v>165</v>
       </c>
-      <c r="B165">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
+      <c r="B166">
+        <v>1</v>
+      </c>
+      <c r="E166">
+        <v>0</v>
+      </c>
+      <c r="F166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
         <v>166</v>
       </c>
-      <c r="B166">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
+      <c r="B167">
+        <v>1</v>
+      </c>
+      <c r="E167">
+        <v>0</v>
+      </c>
+      <c r="F167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
         <v>167</v>
       </c>
-      <c r="B167">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
+      <c r="B168">
+        <v>1</v>
+      </c>
+      <c r="E168">
+        <v>0</v>
+      </c>
+      <c r="F168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
         <v>168</v>
       </c>
-      <c r="B168">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
+      <c r="B169">
+        <v>1</v>
+      </c>
+      <c r="E169">
+        <v>0</v>
+      </c>
+      <c r="F169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
         <v>169</v>
       </c>
-      <c r="B169">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
+      <c r="B170">
+        <v>1</v>
+      </c>
+      <c r="E170">
+        <v>0</v>
+      </c>
+      <c r="F170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
         <v>170</v>
       </c>
-      <c r="B170">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
+      <c r="B171">
+        <v>1</v>
+      </c>
+      <c r="E171">
+        <v>0</v>
+      </c>
+      <c r="F171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
         <v>171</v>
       </c>
-      <c r="B171">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
+      <c r="B172">
+        <v>1</v>
+      </c>
+      <c r="E172">
+        <v>0</v>
+      </c>
+      <c r="F172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
         <v>172</v>
       </c>
-      <c r="B172">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
+      <c r="B173">
+        <v>1</v>
+      </c>
+      <c r="E173">
+        <v>0</v>
+      </c>
+      <c r="F173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
         <v>173</v>
       </c>
-      <c r="B173">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
+      <c r="B174">
+        <v>1</v>
+      </c>
+      <c r="E174">
+        <v>0</v>
+      </c>
+      <c r="F174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
         <v>174</v>
       </c>
-      <c r="B174">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
+      <c r="B175">
+        <v>1</v>
+      </c>
+      <c r="E175">
+        <v>0</v>
+      </c>
+      <c r="F175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
         <v>175</v>
       </c>
-      <c r="B175">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
+      <c r="B176">
+        <v>1</v>
+      </c>
+      <c r="E176">
+        <v>0</v>
+      </c>
+      <c r="F176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
         <v>176</v>
       </c>
-      <c r="B176">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
+      <c r="B177">
+        <v>1</v>
+      </c>
+      <c r="E177">
+        <v>0</v>
+      </c>
+      <c r="F177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
         <v>177</v>
       </c>
-      <c r="B177">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
+      <c r="B178">
+        <v>1</v>
+      </c>
+      <c r="E178">
+        <v>0</v>
+      </c>
+      <c r="F178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
         <v>178</v>
       </c>
-      <c r="B178">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
+      <c r="B179">
+        <v>1</v>
+      </c>
+      <c r="E179">
+        <v>0</v>
+      </c>
+      <c r="F179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
         <v>179</v>
       </c>
-      <c r="B179">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
+      <c r="B180">
+        <v>1</v>
+      </c>
+      <c r="E180">
+        <v>0</v>
+      </c>
+      <c r="F180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
         <v>180</v>
       </c>
-      <c r="B180">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
+      <c r="B181">
+        <v>1</v>
+      </c>
+      <c r="E181">
+        <v>0</v>
+      </c>
+      <c r="F181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
         <v>181</v>
       </c>
-      <c r="B181">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
+      <c r="B182">
+        <v>1</v>
+      </c>
+      <c r="E182">
+        <v>0</v>
+      </c>
+      <c r="F182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
         <v>182</v>
       </c>
-      <c r="B182">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
+      <c r="B183">
+        <v>1</v>
+      </c>
+      <c r="E183">
+        <v>0</v>
+      </c>
+      <c r="F183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
         <v>183</v>
       </c>
-      <c r="B183">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
+      <c r="B184">
+        <v>1</v>
+      </c>
+      <c r="E184">
+        <v>0</v>
+      </c>
+      <c r="F184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
         <v>184</v>
       </c>
-      <c r="B184">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
+      <c r="B185">
+        <v>1</v>
+      </c>
+      <c r="E185">
+        <v>0</v>
+      </c>
+      <c r="F185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
         <v>185</v>
       </c>
-      <c r="B185">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
+      <c r="B186">
+        <v>1</v>
+      </c>
+      <c r="E186">
+        <v>0</v>
+      </c>
+      <c r="F186">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
         <v>186</v>
       </c>
-      <c r="B186">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
+      <c r="B187">
+        <v>1</v>
+      </c>
+      <c r="E187">
+        <v>0</v>
+      </c>
+      <c r="F187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
         <v>187</v>
       </c>
-      <c r="B187">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
+      <c r="B188">
+        <v>1</v>
+      </c>
+      <c r="E188">
+        <v>0</v>
+      </c>
+      <c r="F188">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
         <v>188</v>
       </c>
-      <c r="B188">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
+      <c r="B189">
+        <v>1</v>
+      </c>
+      <c r="E189">
+        <v>0</v>
+      </c>
+      <c r="F189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
         <v>189</v>
       </c>
-      <c r="B189">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
+      <c r="B190">
+        <v>1</v>
+      </c>
+      <c r="E190">
+        <v>0</v>
+      </c>
+      <c r="F190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
         <v>190</v>
       </c>
-      <c r="B190">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
+      <c r="B191">
+        <v>1</v>
+      </c>
+      <c r="E191">
+        <v>0</v>
+      </c>
+      <c r="F191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
         <v>191</v>
       </c>
-      <c r="B191">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
+      <c r="B192">
+        <v>1</v>
+      </c>
+      <c r="E192">
+        <v>0</v>
+      </c>
+      <c r="F192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
         <v>192</v>
       </c>
-      <c r="B192">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
+      <c r="B193">
+        <v>1</v>
+      </c>
+      <c r="E193">
+        <v>0</v>
+      </c>
+      <c r="F193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
         <v>193</v>
       </c>
-      <c r="B193">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
+      <c r="B194">
+        <v>1</v>
+      </c>
+      <c r="E194">
+        <v>0</v>
+      </c>
+      <c r="F194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
         <v>194</v>
       </c>
-      <c r="B194">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
+      <c r="B195">
+        <v>1</v>
+      </c>
+      <c r="E195">
+        <v>0</v>
+      </c>
+      <c r="F195">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
         <v>195</v>
       </c>
-      <c r="B195">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
+      <c r="B196">
+        <v>1</v>
+      </c>
+      <c r="E196">
+        <v>0</v>
+      </c>
+      <c r="F196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
         <v>196</v>
       </c>
-      <c r="B196">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
+      <c r="B197">
+        <v>1</v>
+      </c>
+      <c r="E197">
+        <v>0</v>
+      </c>
+      <c r="F197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
         <v>197</v>
       </c>
-      <c r="B197">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
+      <c r="B198">
+        <v>1</v>
+      </c>
+      <c r="E198">
+        <v>0</v>
+      </c>
+      <c r="F198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
         <v>198</v>
       </c>
-      <c r="B198">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
+      <c r="B199">
+        <v>1</v>
+      </c>
+      <c r="E199">
+        <v>0</v>
+      </c>
+      <c r="F199">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
         <v>199</v>
       </c>
-      <c r="B199">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
+      <c r="B200">
+        <v>1</v>
+      </c>
+      <c r="E200">
+        <v>0</v>
+      </c>
+      <c r="F200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
         <v>200</v>
       </c>
-      <c r="B200">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
+      <c r="B201">
+        <v>1</v>
+      </c>
+      <c r="E201">
+        <v>0</v>
+      </c>
+      <c r="F201">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
         <v>201</v>
       </c>
-      <c r="B201">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
+      <c r="B202">
+        <v>1</v>
+      </c>
+      <c r="E202">
+        <v>0</v>
+      </c>
+      <c r="F202">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
         <v>202</v>
       </c>
-      <c r="B202">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
+      <c r="B203">
+        <v>1</v>
+      </c>
+      <c r="E203">
+        <v>0</v>
+      </c>
+      <c r="F203">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
         <v>203</v>
       </c>
-      <c r="B203">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
+      <c r="B204">
+        <v>1</v>
+      </c>
+      <c r="E204">
+        <v>0</v>
+      </c>
+      <c r="F204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
         <v>204</v>
       </c>
-      <c r="B204">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
+      <c r="B205">
+        <v>1</v>
+      </c>
+      <c r="E205">
+        <v>0</v>
+      </c>
+      <c r="F205">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
         <v>205</v>
       </c>
-      <c r="B205">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
+      <c r="B206">
+        <v>1</v>
+      </c>
+      <c r="E206">
+        <v>0</v>
+      </c>
+      <c r="F206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
         <v>206</v>
       </c>
-      <c r="B206">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
+      <c r="B207">
+        <v>1</v>
+      </c>
+      <c r="E207">
+        <v>0</v>
+      </c>
+      <c r="F207">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
         <v>207</v>
       </c>
-      <c r="B207">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A208" t="s">
+      <c r="B208">
+        <v>1</v>
+      </c>
+      <c r="E208">
+        <v>0</v>
+      </c>
+      <c r="F208">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
         <v>208</v>
       </c>
-      <c r="B208">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
+      <c r="B209">
+        <v>1</v>
+      </c>
+      <c r="E209">
+        <v>0</v>
+      </c>
+      <c r="F209">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
         <v>209</v>
       </c>
-      <c r="B209">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A210" t="s">
+      <c r="B210">
+        <v>1</v>
+      </c>
+      <c r="E210">
+        <v>0</v>
+      </c>
+      <c r="F210">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
         <v>210</v>
       </c>
-      <c r="B210">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
+      <c r="B211">
+        <v>1</v>
+      </c>
+      <c r="E211">
+        <v>0</v>
+      </c>
+      <c r="F211">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
         <v>211</v>
       </c>
-      <c r="B211">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
+      <c r="B212">
+        <v>1</v>
+      </c>
+      <c r="E212">
+        <v>0</v>
+      </c>
+      <c r="F212">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
         <v>212</v>
       </c>
-      <c r="B212">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
+      <c r="B213">
+        <v>1</v>
+      </c>
+      <c r="E213">
+        <v>0</v>
+      </c>
+      <c r="F213">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
         <v>213</v>
       </c>
-      <c r="B213">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A214" t="s">
+      <c r="B214">
+        <v>1</v>
+      </c>
+      <c r="E214">
+        <v>0</v>
+      </c>
+      <c r="F214">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
         <v>214</v>
       </c>
-      <c r="B214">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
+      <c r="B215">
+        <v>1</v>
+      </c>
+      <c r="E215">
+        <v>0</v>
+      </c>
+      <c r="F215">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
         <v>215</v>
       </c>
-      <c r="B215">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A216" t="s">
+      <c r="B216">
+        <v>1</v>
+      </c>
+      <c r="E216">
+        <v>0</v>
+      </c>
+      <c r="F216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
         <v>216</v>
       </c>
-      <c r="B216">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
+      <c r="B217">
+        <v>1</v>
+      </c>
+      <c r="E217">
+        <v>0</v>
+      </c>
+      <c r="F217">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
         <v>217</v>
       </c>
-      <c r="B217">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
+      <c r="B218">
+        <v>1</v>
+      </c>
+      <c r="E218">
+        <v>0</v>
+      </c>
+      <c r="F218">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
         <v>218</v>
       </c>
-      <c r="B218">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A219" t="s">
+      <c r="B219">
+        <v>1</v>
+      </c>
+      <c r="E219">
+        <v>0</v>
+      </c>
+      <c r="F219">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
         <v>219</v>
       </c>
-      <c r="B219">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
+      <c r="B220">
+        <v>1</v>
+      </c>
+      <c r="E220">
+        <v>0</v>
+      </c>
+      <c r="F220">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
         <v>220</v>
       </c>
-      <c r="B220">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
+      <c r="B221">
+        <v>1</v>
+      </c>
+      <c r="E221">
+        <v>0</v>
+      </c>
+      <c r="F221">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
         <v>221</v>
       </c>
-      <c r="B221">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
+      <c r="B222">
+        <v>1</v>
+      </c>
+      <c r="E222">
+        <v>0</v>
+      </c>
+      <c r="F222">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
         <v>222</v>
       </c>
-      <c r="B222">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A223" t="s">
+      <c r="B223">
+        <v>1</v>
+      </c>
+      <c r="E223">
+        <v>0</v>
+      </c>
+      <c r="F223">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
         <v>223</v>
       </c>
-      <c r="B223">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A224" t="s">
+      <c r="B224">
+        <v>1</v>
+      </c>
+      <c r="E224">
+        <v>0</v>
+      </c>
+      <c r="F224">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
         <v>224</v>
       </c>
-      <c r="B224">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A225" t="s">
+      <c r="B225">
+        <v>1</v>
+      </c>
+      <c r="E225">
+        <v>0</v>
+      </c>
+      <c r="F225">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
         <v>225</v>
       </c>
-      <c r="B225">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A226" t="s">
+      <c r="B226">
+        <v>1</v>
+      </c>
+      <c r="E226">
+        <v>0</v>
+      </c>
+      <c r="F226">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
         <v>226</v>
       </c>
-      <c r="B226">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A227" t="s">
+      <c r="B227">
+        <v>1</v>
+      </c>
+      <c r="E227">
+        <v>0</v>
+      </c>
+      <c r="F227">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
         <v>227</v>
       </c>
-      <c r="B227">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A228" t="s">
+      <c r="B228">
+        <v>1</v>
+      </c>
+      <c r="E228">
+        <v>0</v>
+      </c>
+      <c r="F228">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
         <v>228</v>
       </c>
-      <c r="B228">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A229" t="s">
+      <c r="B229">
+        <v>1</v>
+      </c>
+      <c r="E229">
+        <v>0</v>
+      </c>
+      <c r="F229">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
         <v>229</v>
       </c>
-      <c r="B229">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A230" t="s">
-        <v>230</v>
-      </c>
       <c r="B230">
-        <v>3002</v>
+        <v>1</v>
+      </c>
+      <c r="E230">
+        <v>0</v>
+      </c>
+      <c r="F230">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F230">
+    <sortCondition descending="1" ref="B2:B230"/>
+    <sortCondition ref="C2:C230"/>
+    <sortCondition ref="D2:D230"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
corrected group labels on unselected languages
</commit_message>
<xml_diff>
--- a/data/Language sample frequency.xlsx
+++ b/data/Language sample frequency.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\Documents\Utrecht stuff\Pattern Recognition\Accent-Detection\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D632AC-04F4-46D2-9EA6-F44DBD4BCEF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7E0D30-6C5B-4BD0-9518-02ABB2B625DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2955ED82-3F38-426B-B955-560BA7C2C229}"/>
   </bookViews>
@@ -1573,7 +1573,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="12353924" y="1133475"/>
+              <a:off x="12620624" y="1133475"/>
               <a:ext cx="4791075" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">

</xml_diff>